<commit_message>
added icon buttons and some pdf functionality
</commit_message>
<xml_diff>
--- a/InventoryManagementForms/bin/Debug/net6.0-windows/Category.xlsx
+++ b/InventoryManagementForms/bin/Debug/net6.0-windows/Category.xlsx
@@ -23,7 +23,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Category 1</t>
+    <t>testupdateonform</t>
   </si>
   <si>
     <t>Description of category 1</t>
@@ -84,7 +84,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -125,7 +125,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>7</v>
@@ -136,45 +136,12 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="0" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>